<commit_message>
Added Web Scraper Example with Control Rate and Prioritisation
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26722"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26812"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sball/GitHub/nifi-templates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="26940" windowHeight="18640" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="193">
   <si>
     <t>Template Name:</t>
   </si>
@@ -604,6 +609,15 @@
   <si>
     <t>InvokeScriptedProcessor</t>
   </si>
+  <si>
+    <t>Web_Scraper_Sample</t>
+  </si>
+  <si>
+    <t>This template downloads an index of xml documents from an HTML page, then priorises the downloads of different linked pages, and controls the rate of download, before extracting, de-duplicating and routing the results.</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
 </sst>
 </file>
 
@@ -1048,6 +1062,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1376,13 +1395,13 @@
   <dimension ref="A1:DT164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="BJ38" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="J37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="BS4" sqref="BS4"/>
+      <selection pane="bottomRight" activeCell="Q40" sqref="Q40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="40.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="47.5" style="8" customWidth="1"/>
@@ -1393,7 +1412,7 @@
     <col min="124" max="124" width="1.6640625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:124" ht="16" thickBot="1">
+    <row r="1" spans="1:124" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="26" t="s">
         <v>153</v>
       </c>
@@ -1407,11 +1426,11 @@
       </c>
       <c r="F1">
         <f t="shared" ref="F1:L1" si="0">COUNTIFS(F10:F300,"X")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G1">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H1">
         <f t="shared" si="0"/>
@@ -1447,7 +1466,7 @@
       </c>
       <c r="Q1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R1">
         <f t="shared" si="1"/>
@@ -1487,7 +1506,7 @@
       </c>
       <c r="AA1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AB1">
         <f t="shared" si="1"/>
@@ -1511,11 +1530,11 @@
       </c>
       <c r="AG1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH1">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI1">
         <f t="shared" si="1"/>
@@ -1599,7 +1618,7 @@
       </c>
       <c r="BD1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BE1">
         <f t="shared" si="1"/>
@@ -1655,7 +1674,7 @@
       </c>
       <c r="BR1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="BT1">
         <f t="shared" si="1"/>
@@ -1719,7 +1738,7 @@
       </c>
       <c r="CI1">
         <f t="shared" ref="CI1:DS1" si="2">COUNTIFS(CI10:CI300,"X")</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="CJ1">
         <f t="shared" si="2"/>
@@ -1743,7 +1762,7 @@
       </c>
       <c r="CO1">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="CP1">
         <f t="shared" si="2"/>
@@ -1795,7 +1814,7 @@
       </c>
       <c r="DB1">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="DC1">
         <f t="shared" si="2"/>
@@ -1807,7 +1826,7 @@
       </c>
       <c r="DE1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DF1">
         <f t="shared" si="2"/>
@@ -1835,7 +1854,7 @@
       </c>
       <c r="DL1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="DM1">
         <f t="shared" si="2"/>
@@ -1855,7 +1874,7 @@
       </c>
       <c r="DQ1">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="DR1">
         <f t="shared" si="2"/>
@@ -1866,7 +1885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:124" s="5" customFormat="1" ht="48" customHeight="1" thickBot="1">
+    <row r="2" spans="1:124" s="5" customFormat="1" ht="48" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="28" t="s">
         <v>183</v>
       </c>
@@ -1998,7 +2017,7 @@
       <c r="DS2" s="31"/>
       <c r="DT2" s="6"/>
     </row>
-    <row r="3" spans="1:124" s="1" customFormat="1" ht="221" customHeight="1" thickTop="1">
+    <row r="3" spans="1:124" s="1" customFormat="1" ht="221" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="29"/>
       <c r="B3" s="29"/>
       <c r="C3" s="20"/>
@@ -2362,11 +2381,11 @@
       </c>
       <c r="DT3" s="4"/>
     </row>
-    <row r="4" spans="1:124" s="3" customFormat="1" ht="8" customHeight="1">
+    <row r="4" spans="1:124" s="3" customFormat="1" ht="8" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="7"/>
       <c r="C4" s="12"/>
     </row>
-    <row r="5" spans="1:124">
+    <row r="5" spans="1:124" x14ac:dyDescent="0.2">
       <c r="B5" s="8" t="s">
         <v>25</v>
       </c>
@@ -2449,7 +2468,7 @@
       <c r="BV5" s="10"/>
       <c r="BW5" s="10"/>
     </row>
-    <row r="6" spans="1:124">
+    <row r="6" spans="1:124" x14ac:dyDescent="0.2">
       <c r="B6" s="8" t="s">
         <v>26</v>
       </c>
@@ -2538,7 +2557,7 @@
       <c r="BV6" s="10"/>
       <c r="BW6" s="10"/>
     </row>
-    <row r="7" spans="1:124">
+    <row r="7" spans="1:124" x14ac:dyDescent="0.2">
       <c r="B7" s="8" t="s">
         <v>28</v>
       </c>
@@ -2627,7 +2646,7 @@
       <c r="BV7" s="10"/>
       <c r="BW7" s="10"/>
     </row>
-    <row r="8" spans="1:124" s="3" customFormat="1" ht="7" customHeight="1" thickBot="1">
+    <row r="8" spans="1:124" s="3" customFormat="1" ht="7" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="7"/>
       <c r="C8" s="12"/>
       <c r="D8" s="11"/>
@@ -2703,7 +2722,7 @@
       <c r="BV8" s="11"/>
       <c r="BW8" s="11"/>
     </row>
-    <row r="9" spans="1:124" ht="25" customHeight="1" thickTop="1">
+    <row r="9" spans="1:124" ht="25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
         <v>0</v>
       </c>
@@ -2831,7 +2850,7 @@
       <c r="DR9" s="33"/>
       <c r="DS9" s="33"/>
     </row>
-    <row r="10" spans="1:124" ht="120">
+    <row r="10" spans="1:124" ht="128" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
         <v>110</v>
       </c>
@@ -2995,7 +3014,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:124" ht="90">
+    <row r="11" spans="1:124" ht="96" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>111</v>
       </c>
@@ -3135,7 +3154,7 @@
       <c r="DR11" s="13"/>
       <c r="DS11" s="13"/>
     </row>
-    <row r="12" spans="1:124" ht="72" customHeight="1">
+    <row r="12" spans="1:124" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>112</v>
       </c>
@@ -3271,7 +3290,7 @@
       <c r="DR12" s="13"/>
       <c r="DS12" s="13"/>
     </row>
-    <row r="13" spans="1:124" ht="72" customHeight="1">
+    <row r="13" spans="1:124" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>115</v>
       </c>
@@ -3409,7 +3428,7 @@
       <c r="DR13" s="13"/>
       <c r="DS13" s="13"/>
     </row>
-    <row r="14" spans="1:124" ht="90">
+    <row r="14" spans="1:124" ht="96" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>116</v>
       </c>
@@ -3543,7 +3562,7 @@
       <c r="DR14" s="13"/>
       <c r="DS14" s="13"/>
     </row>
-    <row r="15" spans="1:124" ht="90">
+    <row r="15" spans="1:124" ht="96" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>119</v>
       </c>
@@ -3687,7 +3706,7 @@
       <c r="DR15" s="13"/>
       <c r="DS15" s="13"/>
     </row>
-    <row r="16" spans="1:124" ht="72" customHeight="1">
+    <row r="16" spans="1:124" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>122</v>
       </c>
@@ -3827,7 +3846,7 @@
       <c r="DR16" s="13"/>
       <c r="DS16" s="13"/>
     </row>
-    <row r="17" spans="1:123" ht="120">
+    <row r="17" spans="1:123" ht="128" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>123</v>
       </c>
@@ -3965,7 +3984,7 @@
       <c r="DR17" s="13"/>
       <c r="DS17" s="13"/>
     </row>
-    <row r="18" spans="1:123" ht="72" customHeight="1">
+    <row r="18" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>126</v>
       </c>
@@ -4119,7 +4138,7 @@
       <c r="DR18" s="13"/>
       <c r="DS18" s="13"/>
     </row>
-    <row r="19" spans="1:123" ht="72" customHeight="1">
+    <row r="19" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>127</v>
       </c>
@@ -4253,7 +4272,7 @@
       <c r="DR19" s="13"/>
       <c r="DS19" s="13"/>
     </row>
-    <row r="20" spans="1:123" ht="90">
+    <row r="20" spans="1:123" ht="96" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>128</v>
       </c>
@@ -4385,7 +4404,7 @@
       <c r="DR20" s="13"/>
       <c r="DS20" s="13"/>
     </row>
-    <row r="21" spans="1:123" ht="72" customHeight="1">
+    <row r="21" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>131</v>
       </c>
@@ -4521,7 +4540,7 @@
       <c r="DR21" s="13"/>
       <c r="DS21" s="13"/>
     </row>
-    <row r="22" spans="1:123" ht="105">
+    <row r="22" spans="1:123" ht="112" x14ac:dyDescent="0.2">
       <c r="A22" s="22" t="s">
         <v>133</v>
       </c>
@@ -4661,7 +4680,7 @@
       <c r="DR22" s="13"/>
       <c r="DS22" s="13"/>
     </row>
-    <row r="23" spans="1:123" ht="105">
+    <row r="23" spans="1:123" ht="112" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
         <v>136</v>
       </c>
@@ -4799,7 +4818,7 @@
       <c r="DR23" s="13"/>
       <c r="DS23" s="13"/>
     </row>
-    <row r="24" spans="1:123" ht="120">
+    <row r="24" spans="1:123" ht="128" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>138</v>
       </c>
@@ -4933,7 +4952,7 @@
       <c r="DR24" s="13"/>
       <c r="DS24" s="13"/>
     </row>
-    <row r="25" spans="1:123" ht="75">
+    <row r="25" spans="1:123" ht="80" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>140</v>
       </c>
@@ -5069,7 +5088,7 @@
       <c r="DR25" s="13"/>
       <c r="DS25" s="13"/>
     </row>
-    <row r="26" spans="1:123" ht="240">
+    <row r="26" spans="1:123" ht="256" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>142</v>
       </c>
@@ -5211,7 +5230,7 @@
       <c r="DR26" s="13"/>
       <c r="DS26" s="13"/>
     </row>
-    <row r="27" spans="1:123" ht="330">
+    <row r="27" spans="1:123" ht="352" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>144</v>
       </c>
@@ -5347,7 +5366,7 @@
       <c r="DR27" s="13"/>
       <c r="DS27" s="13"/>
     </row>
-    <row r="28" spans="1:123" ht="409">
+    <row r="28" spans="1:123" ht="409" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>147</v>
       </c>
@@ -5495,7 +5514,7 @@
       <c r="DR28" s="13"/>
       <c r="DS28" s="13"/>
     </row>
-    <row r="29" spans="1:123" ht="72" customHeight="1">
+    <row r="29" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>163</v>
       </c>
@@ -5633,7 +5652,7 @@
       <c r="DR29" s="13"/>
       <c r="DS29" s="13"/>
     </row>
-    <row r="30" spans="1:123" ht="105">
+    <row r="30" spans="1:123" ht="112" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
         <v>165</v>
       </c>
@@ -5777,7 +5796,7 @@
       <c r="DR30" s="13"/>
       <c r="DS30" s="13"/>
     </row>
-    <row r="31" spans="1:123" ht="165">
+    <row r="31" spans="1:123" ht="176" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>168</v>
       </c>
@@ -5937,7 +5956,7 @@
       <c r="DR31" s="13"/>
       <c r="DS31" s="13"/>
     </row>
-    <row r="32" spans="1:123" ht="72" customHeight="1">
+    <row r="32" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
         <v>169</v>
       </c>
@@ -6075,7 +6094,7 @@
       <c r="DR32" s="13"/>
       <c r="DS32" s="13"/>
     </row>
-    <row r="33" spans="1:123" ht="72" customHeight="1">
+    <row r="33" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="22" t="s">
         <v>171</v>
       </c>
@@ -6211,7 +6230,7 @@
       <c r="DR33" s="13"/>
       <c r="DS33" s="13"/>
     </row>
-    <row r="34" spans="1:123" ht="72" customHeight="1">
+    <row r="34" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>173</v>
       </c>
@@ -6355,7 +6374,7 @@
       <c r="DR34" s="13"/>
       <c r="DS34" s="13"/>
     </row>
-    <row r="35" spans="1:123" ht="72" customHeight="1">
+    <row r="35" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
         <v>175</v>
       </c>
@@ -6513,7 +6532,7 @@
       <c r="DR35" s="13"/>
       <c r="DS35" s="13"/>
     </row>
-    <row r="36" spans="1:123" ht="72" customHeight="1">
+    <row r="36" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
         <v>178</v>
       </c>
@@ -6657,7 +6676,7 @@
       <c r="DR36" s="13"/>
       <c r="DS36" s="13"/>
     </row>
-    <row r="37" spans="1:123" ht="72" customHeight="1">
+    <row r="37" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
         <v>179</v>
       </c>
@@ -6805,7 +6824,7 @@
       <c r="DR37" s="13"/>
       <c r="DS37" s="13"/>
     </row>
-    <row r="38" spans="1:123" ht="72" customHeight="1">
+    <row r="38" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="22" t="s">
         <v>184</v>
       </c>
@@ -6943,7 +6962,7 @@
       <c r="DR38" s="13"/>
       <c r="DS38" s="13"/>
     </row>
-    <row r="39" spans="1:123" ht="72" customHeight="1">
+    <row r="39" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
         <v>186</v>
       </c>
@@ -7081,13 +7100,21 @@
       <c r="DR39" s="13"/>
       <c r="DS39" s="13"/>
     </row>
-    <row r="40" spans="1:123" ht="72" customHeight="1">
-      <c r="A40" s="16"/>
-      <c r="B40" s="24"/>
+    <row r="40" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B40" s="24" t="s">
+        <v>191</v>
+      </c>
       <c r="D40" s="18"/>
       <c r="E40" s="18"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
+      <c r="F40" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="G40" s="13" t="s">
+        <v>192</v>
+      </c>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
@@ -7097,7 +7124,9 @@
       <c r="N40" s="13"/>
       <c r="O40" s="13"/>
       <c r="P40" s="13"/>
-      <c r="Q40" s="13"/>
+      <c r="Q40" s="13" t="s">
+        <v>192</v>
+      </c>
       <c r="R40" s="13"/>
       <c r="S40" s="13"/>
       <c r="T40" s="13"/>
@@ -7107,14 +7136,20 @@
       <c r="X40" s="13"/>
       <c r="Y40" s="13"/>
       <c r="Z40" s="13"/>
-      <c r="AA40" s="13"/>
+      <c r="AA40" s="13" t="s">
+        <v>192</v>
+      </c>
       <c r="AB40" s="13"/>
       <c r="AC40" s="13"/>
       <c r="AD40" s="13"/>
       <c r="AE40" s="13"/>
       <c r="AF40" s="13"/>
-      <c r="AG40" s="13"/>
-      <c r="AH40" s="13"/>
+      <c r="AG40" s="13" t="s">
+        <v>192</v>
+      </c>
+      <c r="AH40" s="13" t="s">
+        <v>192</v>
+      </c>
       <c r="AI40" s="13"/>
       <c r="AJ40" s="13"/>
       <c r="AK40" s="13"/>
@@ -7136,7 +7171,9 @@
       <c r="BA40" s="13"/>
       <c r="BB40" s="13"/>
       <c r="BC40" s="13"/>
-      <c r="BD40" s="13"/>
+      <c r="BD40" s="13" t="s">
+        <v>192</v>
+      </c>
       <c r="BE40" s="13"/>
       <c r="BF40" s="13"/>
       <c r="BG40" s="13"/>
@@ -7150,7 +7187,9 @@
       <c r="BO40" s="13"/>
       <c r="BP40" s="13"/>
       <c r="BQ40" s="13"/>
-      <c r="BR40" s="13"/>
+      <c r="BR40" s="13" t="s">
+        <v>192</v>
+      </c>
       <c r="BS40" s="13"/>
       <c r="BT40" s="13"/>
       <c r="BU40" s="13"/>
@@ -7167,13 +7206,17 @@
       <c r="CF40" s="13"/>
       <c r="CG40" s="13"/>
       <c r="CH40" s="13"/>
-      <c r="CI40" s="13"/>
+      <c r="CI40" s="13" t="s">
+        <v>192</v>
+      </c>
       <c r="CJ40" s="13"/>
       <c r="CK40" s="13"/>
       <c r="CL40" s="13"/>
       <c r="CM40" s="13"/>
       <c r="CN40" s="13"/>
-      <c r="CO40" s="13"/>
+      <c r="CO40" s="13" t="s">
+        <v>192</v>
+      </c>
       <c r="CP40" s="13"/>
       <c r="CQ40" s="13"/>
       <c r="CR40" s="13"/>
@@ -7186,26 +7229,34 @@
       <c r="CY40" s="13"/>
       <c r="CZ40" s="13"/>
       <c r="DA40" s="13"/>
-      <c r="DB40" s="13"/>
+      <c r="DB40" s="13" t="s">
+        <v>192</v>
+      </c>
       <c r="DC40" s="13"/>
       <c r="DD40" s="13"/>
-      <c r="DE40" s="13"/>
+      <c r="DE40" s="13" t="s">
+        <v>192</v>
+      </c>
       <c r="DF40" s="13"/>
       <c r="DG40" s="13"/>
       <c r="DH40" s="13"/>
       <c r="DI40" s="13"/>
       <c r="DJ40" s="13"/>
       <c r="DK40" s="13"/>
-      <c r="DL40" s="13"/>
+      <c r="DL40" s="13" t="s">
+        <v>192</v>
+      </c>
       <c r="DM40" s="13"/>
       <c r="DN40" s="13"/>
       <c r="DO40" s="13"/>
       <c r="DP40" s="13"/>
-      <c r="DQ40" s="13"/>
+      <c r="DQ40" s="13" t="s">
+        <v>192</v>
+      </c>
       <c r="DR40" s="13"/>
       <c r="DS40" s="13"/>
     </row>
-    <row r="41" spans="1:123" ht="72" customHeight="1">
+    <row r="41" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="16"/>
       <c r="B41" s="24"/>
       <c r="D41" s="18"/>
@@ -7329,7 +7380,7 @@
       <c r="DR41" s="13"/>
       <c r="DS41" s="13"/>
     </row>
-    <row r="42" spans="1:123" ht="72" customHeight="1">
+    <row r="42" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="16"/>
       <c r="B42" s="24"/>
       <c r="D42" s="18"/>
@@ -7453,7 +7504,7 @@
       <c r="DR42" s="13"/>
       <c r="DS42" s="13"/>
     </row>
-    <row r="43" spans="1:123" ht="72" customHeight="1">
+    <row r="43" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="16"/>
       <c r="B43" s="24"/>
       <c r="D43" s="18"/>
@@ -7577,7 +7628,7 @@
       <c r="DR43" s="13"/>
       <c r="DS43" s="13"/>
     </row>
-    <row r="44" spans="1:123" ht="72" customHeight="1">
+    <row r="44" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="16"/>
       <c r="B44" s="24"/>
       <c r="D44" s="18"/>
@@ -7701,7 +7752,7 @@
       <c r="DR44" s="13"/>
       <c r="DS44" s="13"/>
     </row>
-    <row r="45" spans="1:123" ht="72" customHeight="1">
+    <row r="45" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="16"/>
       <c r="B45" s="24"/>
       <c r="D45" s="18"/>
@@ -7825,7 +7876,7 @@
       <c r="DR45" s="13"/>
       <c r="DS45" s="13"/>
     </row>
-    <row r="46" spans="1:123" ht="72" customHeight="1">
+    <row r="46" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="16"/>
       <c r="B46" s="24"/>
       <c r="D46" s="18"/>
@@ -7949,7 +8000,7 @@
       <c r="DR46" s="13"/>
       <c r="DS46" s="13"/>
     </row>
-    <row r="47" spans="1:123" ht="72" customHeight="1">
+    <row r="47" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="16"/>
       <c r="B47" s="24"/>
       <c r="D47" s="18"/>
@@ -8073,7 +8124,7 @@
       <c r="DR47" s="13"/>
       <c r="DS47" s="13"/>
     </row>
-    <row r="48" spans="1:123" ht="72" customHeight="1">
+    <row r="48" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="16"/>
       <c r="B48" s="24"/>
       <c r="D48" s="18"/>
@@ -8197,7 +8248,7 @@
       <c r="DR48" s="13"/>
       <c r="DS48" s="13"/>
     </row>
-    <row r="49" spans="1:123" ht="72" customHeight="1">
+    <row r="49" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="16"/>
       <c r="B49" s="24"/>
       <c r="D49" s="18"/>
@@ -8321,7 +8372,7 @@
       <c r="DR49" s="13"/>
       <c r="DS49" s="13"/>
     </row>
-    <row r="50" spans="1:123" ht="72" customHeight="1">
+    <row r="50" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="16"/>
       <c r="B50" s="24"/>
       <c r="D50" s="18"/>
@@ -8445,7 +8496,7 @@
       <c r="DR50" s="13"/>
       <c r="DS50" s="13"/>
     </row>
-    <row r="51" spans="1:123" ht="72" customHeight="1">
+    <row r="51" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="16"/>
       <c r="B51" s="24"/>
       <c r="D51" s="18"/>
@@ -8569,7 +8620,7 @@
       <c r="DR51" s="13"/>
       <c r="DS51" s="13"/>
     </row>
-    <row r="52" spans="1:123" ht="72" customHeight="1">
+    <row r="52" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="16"/>
       <c r="B52" s="24"/>
       <c r="D52" s="18"/>
@@ -8693,7 +8744,7 @@
       <c r="DR52" s="13"/>
       <c r="DS52" s="13"/>
     </row>
-    <row r="53" spans="1:123" ht="72" customHeight="1">
+    <row r="53" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="16"/>
       <c r="B53" s="24"/>
       <c r="D53" s="18"/>
@@ -8817,7 +8868,7 @@
       <c r="DR53" s="13"/>
       <c r="DS53" s="13"/>
     </row>
-    <row r="54" spans="1:123" ht="72" customHeight="1">
+    <row r="54" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="16"/>
       <c r="B54" s="24"/>
       <c r="D54" s="18"/>
@@ -8941,7 +8992,7 @@
       <c r="DR54" s="13"/>
       <c r="DS54" s="13"/>
     </row>
-    <row r="55" spans="1:123" ht="72" customHeight="1">
+    <row r="55" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="16"/>
       <c r="B55" s="24"/>
       <c r="D55" s="18"/>
@@ -9065,7 +9116,7 @@
       <c r="DR55" s="13"/>
       <c r="DS55" s="13"/>
     </row>
-    <row r="56" spans="1:123" ht="72" customHeight="1">
+    <row r="56" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="16"/>
       <c r="B56" s="24"/>
       <c r="D56" s="18"/>
@@ -9189,7 +9240,7 @@
       <c r="DR56" s="13"/>
       <c r="DS56" s="13"/>
     </row>
-    <row r="57" spans="1:123" ht="72" customHeight="1">
+    <row r="57" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="16"/>
       <c r="B57" s="24"/>
       <c r="D57" s="18"/>
@@ -9313,7 +9364,7 @@
       <c r="DR57" s="13"/>
       <c r="DS57" s="13"/>
     </row>
-    <row r="58" spans="1:123" ht="72" customHeight="1">
+    <row r="58" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="16"/>
       <c r="B58" s="24"/>
       <c r="D58" s="18"/>
@@ -9437,7 +9488,7 @@
       <c r="DR58" s="13"/>
       <c r="DS58" s="13"/>
     </row>
-    <row r="59" spans="1:123" ht="72" customHeight="1">
+    <row r="59" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="16"/>
       <c r="B59" s="24"/>
       <c r="D59" s="18"/>
@@ -9561,7 +9612,7 @@
       <c r="DR59" s="13"/>
       <c r="DS59" s="13"/>
     </row>
-    <row r="60" spans="1:123" ht="72" customHeight="1">
+    <row r="60" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="16"/>
       <c r="B60" s="24"/>
       <c r="D60" s="18"/>
@@ -9685,7 +9736,7 @@
       <c r="DR60" s="13"/>
       <c r="DS60" s="13"/>
     </row>
-    <row r="61" spans="1:123" ht="72" customHeight="1">
+    <row r="61" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="16"/>
       <c r="B61" s="24"/>
       <c r="D61" s="18"/>
@@ -9809,7 +9860,7 @@
       <c r="DR61" s="13"/>
       <c r="DS61" s="13"/>
     </row>
-    <row r="62" spans="1:123" ht="72" customHeight="1">
+    <row r="62" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="16"/>
       <c r="B62" s="24"/>
       <c r="D62" s="18"/>
@@ -9933,7 +9984,7 @@
       <c r="DR62" s="13"/>
       <c r="DS62" s="13"/>
     </row>
-    <row r="63" spans="1:123" ht="72" customHeight="1">
+    <row r="63" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="16"/>
       <c r="B63" s="24"/>
       <c r="D63" s="18"/>
@@ -10057,7 +10108,7 @@
       <c r="DR63" s="13"/>
       <c r="DS63" s="13"/>
     </row>
-    <row r="64" spans="1:123" ht="72" customHeight="1">
+    <row r="64" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="16"/>
       <c r="B64" s="24"/>
       <c r="D64" s="18"/>
@@ -10181,7 +10232,7 @@
       <c r="DR64" s="13"/>
       <c r="DS64" s="13"/>
     </row>
-    <row r="65" spans="1:123" ht="72" customHeight="1">
+    <row r="65" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="16"/>
       <c r="B65" s="24"/>
       <c r="D65" s="18"/>
@@ -10305,7 +10356,7 @@
       <c r="DR65" s="13"/>
       <c r="DS65" s="13"/>
     </row>
-    <row r="66" spans="1:123" ht="72" customHeight="1">
+    <row r="66" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="16"/>
       <c r="B66" s="24"/>
       <c r="D66" s="18"/>
@@ -10429,7 +10480,7 @@
       <c r="DR66" s="13"/>
       <c r="DS66" s="13"/>
     </row>
-    <row r="67" spans="1:123" ht="72" customHeight="1">
+    <row r="67" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="16"/>
       <c r="B67" s="24"/>
       <c r="D67" s="18"/>
@@ -10553,7 +10604,7 @@
       <c r="DR67" s="13"/>
       <c r="DS67" s="13"/>
     </row>
-    <row r="68" spans="1:123" ht="72" customHeight="1">
+    <row r="68" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="16"/>
       <c r="B68" s="24"/>
       <c r="D68" s="18"/>
@@ -10677,7 +10728,7 @@
       <c r="DR68" s="13"/>
       <c r="DS68" s="13"/>
     </row>
-    <row r="69" spans="1:123" ht="72" customHeight="1">
+    <row r="69" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="16"/>
       <c r="B69" s="24"/>
       <c r="D69" s="18"/>
@@ -10801,7 +10852,7 @@
       <c r="DR69" s="13"/>
       <c r="DS69" s="13"/>
     </row>
-    <row r="70" spans="1:123" ht="72" customHeight="1">
+    <row r="70" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="16"/>
       <c r="B70" s="24"/>
       <c r="D70" s="18"/>
@@ -10925,7 +10976,7 @@
       <c r="DR70" s="13"/>
       <c r="DS70" s="13"/>
     </row>
-    <row r="71" spans="1:123" ht="72" customHeight="1">
+    <row r="71" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="16"/>
       <c r="B71" s="24"/>
       <c r="D71" s="18"/>
@@ -11049,7 +11100,7 @@
       <c r="DR71" s="13"/>
       <c r="DS71" s="13"/>
     </row>
-    <row r="72" spans="1:123" ht="72" customHeight="1">
+    <row r="72" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="16"/>
       <c r="B72" s="24"/>
       <c r="D72" s="18"/>
@@ -11173,7 +11224,7 @@
       <c r="DR72" s="13"/>
       <c r="DS72" s="13"/>
     </row>
-    <row r="73" spans="1:123" ht="72" customHeight="1">
+    <row r="73" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="16"/>
       <c r="B73" s="24"/>
       <c r="D73" s="18"/>
@@ -11297,7 +11348,7 @@
       <c r="DR73" s="13"/>
       <c r="DS73" s="13"/>
     </row>
-    <row r="74" spans="1:123" ht="72" customHeight="1">
+    <row r="74" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="16"/>
       <c r="B74" s="24"/>
       <c r="D74" s="18"/>
@@ -11421,7 +11472,7 @@
       <c r="DR74" s="13"/>
       <c r="DS74" s="13"/>
     </row>
-    <row r="75" spans="1:123" ht="72" customHeight="1">
+    <row r="75" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="16"/>
       <c r="B75" s="24"/>
       <c r="D75" s="18"/>
@@ -11545,7 +11596,7 @@
       <c r="DR75" s="13"/>
       <c r="DS75" s="13"/>
     </row>
-    <row r="76" spans="1:123" ht="72" customHeight="1">
+    <row r="76" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="16"/>
       <c r="B76" s="24"/>
       <c r="D76" s="18"/>
@@ -11669,7 +11720,7 @@
       <c r="DR76" s="13"/>
       <c r="DS76" s="13"/>
     </row>
-    <row r="77" spans="1:123" ht="72" customHeight="1">
+    <row r="77" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="16"/>
       <c r="B77" s="24"/>
       <c r="D77" s="18"/>
@@ -11793,7 +11844,7 @@
       <c r="DR77" s="13"/>
       <c r="DS77" s="13"/>
     </row>
-    <row r="78" spans="1:123" ht="72" customHeight="1">
+    <row r="78" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="16"/>
       <c r="B78" s="24"/>
       <c r="D78" s="18"/>
@@ -11917,7 +11968,7 @@
       <c r="DR78" s="13"/>
       <c r="DS78" s="13"/>
     </row>
-    <row r="79" spans="1:123" ht="72" customHeight="1">
+    <row r="79" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="16"/>
       <c r="B79" s="24"/>
       <c r="D79" s="18"/>
@@ -12041,7 +12092,7 @@
       <c r="DR79" s="13"/>
       <c r="DS79" s="13"/>
     </row>
-    <row r="80" spans="1:123" ht="72" customHeight="1">
+    <row r="80" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="16"/>
       <c r="B80" s="24"/>
       <c r="D80" s="18"/>
@@ -12165,7 +12216,7 @@
       <c r="DR80" s="13"/>
       <c r="DS80" s="13"/>
     </row>
-    <row r="81" spans="1:123" ht="72" customHeight="1">
+    <row r="81" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="16"/>
       <c r="B81" s="24"/>
       <c r="D81" s="18"/>
@@ -12289,7 +12340,7 @@
       <c r="DR81" s="13"/>
       <c r="DS81" s="13"/>
     </row>
-    <row r="82" spans="1:123" ht="72" customHeight="1">
+    <row r="82" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="16"/>
       <c r="B82" s="24"/>
       <c r="D82" s="18"/>
@@ -12413,7 +12464,7 @@
       <c r="DR82" s="13"/>
       <c r="DS82" s="13"/>
     </row>
-    <row r="83" spans="1:123" ht="72" customHeight="1">
+    <row r="83" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="16"/>
       <c r="B83" s="24"/>
       <c r="D83" s="18"/>
@@ -12537,7 +12588,7 @@
       <c r="DR83" s="13"/>
       <c r="DS83" s="13"/>
     </row>
-    <row r="84" spans="1:123" ht="72" customHeight="1">
+    <row r="84" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="16"/>
       <c r="B84" s="24"/>
       <c r="D84" s="18"/>
@@ -12661,7 +12712,7 @@
       <c r="DR84" s="13"/>
       <c r="DS84" s="13"/>
     </row>
-    <row r="85" spans="1:123" ht="72" customHeight="1">
+    <row r="85" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="16"/>
       <c r="B85" s="24"/>
       <c r="D85" s="18"/>
@@ -12785,7 +12836,7 @@
       <c r="DR85" s="13"/>
       <c r="DS85" s="13"/>
     </row>
-    <row r="86" spans="1:123" ht="72" customHeight="1">
+    <row r="86" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="16"/>
       <c r="B86" s="24"/>
       <c r="D86" s="18"/>
@@ -12909,7 +12960,7 @@
       <c r="DR86" s="13"/>
       <c r="DS86" s="13"/>
     </row>
-    <row r="87" spans="1:123" ht="72" customHeight="1">
+    <row r="87" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="16"/>
       <c r="B87" s="24"/>
       <c r="D87" s="18"/>
@@ -13033,7 +13084,7 @@
       <c r="DR87" s="13"/>
       <c r="DS87" s="13"/>
     </row>
-    <row r="88" spans="1:123" ht="72" customHeight="1">
+    <row r="88" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="16"/>
       <c r="B88" s="24"/>
       <c r="D88" s="18"/>
@@ -13157,7 +13208,7 @@
       <c r="DR88" s="13"/>
       <c r="DS88" s="13"/>
     </row>
-    <row r="89" spans="1:123" ht="72" customHeight="1">
+    <row r="89" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="16"/>
       <c r="B89" s="24"/>
       <c r="D89" s="18"/>
@@ -13281,7 +13332,7 @@
       <c r="DR89" s="13"/>
       <c r="DS89" s="13"/>
     </row>
-    <row r="90" spans="1:123" ht="72" customHeight="1">
+    <row r="90" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="16"/>
       <c r="B90" s="24"/>
       <c r="D90" s="18"/>
@@ -13405,7 +13456,7 @@
       <c r="DR90" s="13"/>
       <c r="DS90" s="13"/>
     </row>
-    <row r="91" spans="1:123" ht="72" customHeight="1">
+    <row r="91" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="16"/>
       <c r="B91" s="24"/>
       <c r="D91" s="18"/>
@@ -13529,7 +13580,7 @@
       <c r="DR91" s="13"/>
       <c r="DS91" s="13"/>
     </row>
-    <row r="92" spans="1:123" ht="72" customHeight="1">
+    <row r="92" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="16"/>
       <c r="B92" s="24"/>
       <c r="D92" s="18"/>
@@ -13653,7 +13704,7 @@
       <c r="DR92" s="13"/>
       <c r="DS92" s="13"/>
     </row>
-    <row r="93" spans="1:123" ht="72" customHeight="1">
+    <row r="93" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="16"/>
       <c r="B93" s="24"/>
       <c r="D93" s="18"/>
@@ -13777,7 +13828,7 @@
       <c r="DR93" s="13"/>
       <c r="DS93" s="13"/>
     </row>
-    <row r="94" spans="1:123" ht="72" customHeight="1">
+    <row r="94" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="16"/>
       <c r="B94" s="24"/>
       <c r="D94" s="18"/>
@@ -13901,7 +13952,7 @@
       <c r="DR94" s="13"/>
       <c r="DS94" s="13"/>
     </row>
-    <row r="95" spans="1:123" ht="72" customHeight="1">
+    <row r="95" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="16"/>
       <c r="B95" s="24"/>
       <c r="D95" s="18"/>
@@ -14025,7 +14076,7 @@
       <c r="DR95" s="13"/>
       <c r="DS95" s="13"/>
     </row>
-    <row r="96" spans="1:123" ht="72" customHeight="1">
+    <row r="96" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="16"/>
       <c r="B96" s="24"/>
       <c r="D96" s="18"/>
@@ -14149,7 +14200,7 @@
       <c r="DR96" s="13"/>
       <c r="DS96" s="13"/>
     </row>
-    <row r="97" spans="1:123" ht="72" customHeight="1">
+    <row r="97" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="16"/>
       <c r="B97" s="24"/>
       <c r="D97" s="18"/>
@@ -14273,7 +14324,7 @@
       <c r="DR97" s="13"/>
       <c r="DS97" s="13"/>
     </row>
-    <row r="98" spans="1:123" ht="72" customHeight="1">
+    <row r="98" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="16"/>
       <c r="B98" s="24"/>
       <c r="D98" s="18"/>
@@ -14397,7 +14448,7 @@
       <c r="DR98" s="13"/>
       <c r="DS98" s="13"/>
     </row>
-    <row r="99" spans="1:123" ht="72" customHeight="1">
+    <row r="99" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="16"/>
       <c r="B99" s="24"/>
       <c r="D99" s="18"/>
@@ -14521,7 +14572,7 @@
       <c r="DR99" s="13"/>
       <c r="DS99" s="13"/>
     </row>
-    <row r="100" spans="1:123" ht="72" customHeight="1">
+    <row r="100" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="16"/>
       <c r="B100" s="24"/>
       <c r="D100" s="18"/>
@@ -14645,7 +14696,7 @@
       <c r="DR100" s="13"/>
       <c r="DS100" s="13"/>
     </row>
-    <row r="101" spans="1:123" ht="72" customHeight="1">
+    <row r="101" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="16"/>
       <c r="B101" s="24"/>
       <c r="D101" s="18"/>
@@ -14769,7 +14820,7 @@
       <c r="DR101" s="13"/>
       <c r="DS101" s="13"/>
     </row>
-    <row r="102" spans="1:123" ht="72" customHeight="1">
+    <row r="102" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="16"/>
       <c r="B102" s="24"/>
       <c r="D102" s="18"/>
@@ -14893,7 +14944,7 @@
       <c r="DR102" s="13"/>
       <c r="DS102" s="13"/>
     </row>
-    <row r="103" spans="1:123" ht="72" customHeight="1">
+    <row r="103" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="16"/>
       <c r="B103" s="24"/>
       <c r="D103" s="18"/>
@@ -15017,7 +15068,7 @@
       <c r="DR103" s="13"/>
       <c r="DS103" s="13"/>
     </row>
-    <row r="104" spans="1:123" ht="72" customHeight="1">
+    <row r="104" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="16"/>
       <c r="B104" s="24"/>
       <c r="D104" s="18"/>
@@ -15141,7 +15192,7 @@
       <c r="DR104" s="13"/>
       <c r="DS104" s="13"/>
     </row>
-    <row r="105" spans="1:123" ht="72" customHeight="1">
+    <row r="105" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="16"/>
       <c r="B105" s="24"/>
       <c r="D105" s="18"/>
@@ -15265,7 +15316,7 @@
       <c r="DR105" s="13"/>
       <c r="DS105" s="13"/>
     </row>
-    <row r="106" spans="1:123" ht="72" customHeight="1">
+    <row r="106" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="16"/>
       <c r="B106" s="24"/>
       <c r="D106" s="18"/>
@@ -15389,7 +15440,7 @@
       <c r="DR106" s="13"/>
       <c r="DS106" s="13"/>
     </row>
-    <row r="107" spans="1:123" ht="72" customHeight="1">
+    <row r="107" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="16"/>
       <c r="B107" s="24"/>
       <c r="D107" s="18"/>
@@ -15513,7 +15564,7 @@
       <c r="DR107" s="13"/>
       <c r="DS107" s="13"/>
     </row>
-    <row r="108" spans="1:123" ht="72" customHeight="1">
+    <row r="108" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="16"/>
       <c r="B108" s="24"/>
       <c r="D108" s="18"/>
@@ -15637,7 +15688,7 @@
       <c r="DR108" s="13"/>
       <c r="DS108" s="13"/>
     </row>
-    <row r="109" spans="1:123" ht="72" customHeight="1">
+    <row r="109" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="16"/>
       <c r="B109" s="24"/>
       <c r="D109" s="18"/>
@@ -15761,7 +15812,7 @@
       <c r="DR109" s="13"/>
       <c r="DS109" s="13"/>
     </row>
-    <row r="110" spans="1:123" ht="72" customHeight="1">
+    <row r="110" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="16"/>
       <c r="B110" s="24"/>
       <c r="D110" s="18"/>
@@ -15885,7 +15936,7 @@
       <c r="DR110" s="13"/>
       <c r="DS110" s="13"/>
     </row>
-    <row r="111" spans="1:123" ht="72" customHeight="1">
+    <row r="111" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="16"/>
       <c r="B111" s="24"/>
       <c r="D111" s="18"/>
@@ -16009,7 +16060,7 @@
       <c r="DR111" s="13"/>
       <c r="DS111" s="13"/>
     </row>
-    <row r="112" spans="1:123" ht="72" customHeight="1">
+    <row r="112" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="16"/>
       <c r="B112" s="24"/>
       <c r="D112" s="18"/>
@@ -16133,7 +16184,7 @@
       <c r="DR112" s="13"/>
       <c r="DS112" s="13"/>
     </row>
-    <row r="113" spans="1:123" ht="72" customHeight="1">
+    <row r="113" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="16"/>
       <c r="B113" s="24"/>
       <c r="D113" s="18"/>
@@ -16257,7 +16308,7 @@
       <c r="DR113" s="13"/>
       <c r="DS113" s="13"/>
     </row>
-    <row r="114" spans="1:123" ht="72" customHeight="1">
+    <row r="114" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="16"/>
       <c r="B114" s="24"/>
       <c r="D114" s="18"/>
@@ -16381,7 +16432,7 @@
       <c r="DR114" s="13"/>
       <c r="DS114" s="13"/>
     </row>
-    <row r="115" spans="1:123" ht="72" customHeight="1">
+    <row r="115" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="16"/>
       <c r="B115" s="24"/>
       <c r="D115" s="18"/>
@@ -16505,7 +16556,7 @@
       <c r="DR115" s="13"/>
       <c r="DS115" s="13"/>
     </row>
-    <row r="116" spans="1:123" ht="72" customHeight="1">
+    <row r="116" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="16"/>
       <c r="B116" s="24"/>
       <c r="D116" s="18"/>
@@ -16629,7 +16680,7 @@
       <c r="DR116" s="13"/>
       <c r="DS116" s="13"/>
     </row>
-    <row r="117" spans="1:123" ht="72" customHeight="1">
+    <row r="117" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B117" s="25"/>
       <c r="D117" s="10"/>
       <c r="E117" s="21"/>
@@ -16704,7 +16755,7 @@
       <c r="BV117" s="10"/>
       <c r="BW117" s="10"/>
     </row>
-    <row r="118" spans="1:123" ht="72" customHeight="1">
+    <row r="118" spans="1:123" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B118" s="25"/>
       <c r="D118" s="10"/>
       <c r="E118" s="21"/>
@@ -16779,7 +16830,7 @@
       <c r="BV118" s="10"/>
       <c r="BW118" s="10"/>
     </row>
-    <row r="119" spans="1:123">
+    <row r="119" spans="1:123" x14ac:dyDescent="0.2">
       <c r="B119" s="25"/>
       <c r="D119" s="10"/>
       <c r="E119" s="21"/>
@@ -16854,7 +16905,7 @@
       <c r="BV119" s="10"/>
       <c r="BW119" s="10"/>
     </row>
-    <row r="120" spans="1:123">
+    <row r="120" spans="1:123" x14ac:dyDescent="0.2">
       <c r="B120" s="25"/>
       <c r="D120" s="10"/>
       <c r="E120" s="21"/>
@@ -16929,7 +16980,7 @@
       <c r="BV120" s="10"/>
       <c r="BW120" s="10"/>
     </row>
-    <row r="121" spans="1:123">
+    <row r="121" spans="1:123" x14ac:dyDescent="0.2">
       <c r="B121" s="25"/>
       <c r="D121" s="10"/>
       <c r="E121" s="21"/>
@@ -17004,7 +17055,7 @@
       <c r="BV121" s="10"/>
       <c r="BW121" s="10"/>
     </row>
-    <row r="122" spans="1:123">
+    <row r="122" spans="1:123" x14ac:dyDescent="0.2">
       <c r="B122" s="25"/>
       <c r="D122" s="10"/>
       <c r="E122" s="21"/>
@@ -17079,7 +17130,7 @@
       <c r="BV122" s="10"/>
       <c r="BW122" s="10"/>
     </row>
-    <row r="123" spans="1:123">
+    <row r="123" spans="1:123" x14ac:dyDescent="0.2">
       <c r="B123" s="25"/>
       <c r="D123" s="10"/>
       <c r="E123" s="21"/>
@@ -17154,7 +17205,7 @@
       <c r="BV123" s="10"/>
       <c r="BW123" s="10"/>
     </row>
-    <row r="124" spans="1:123">
+    <row r="124" spans="1:123" x14ac:dyDescent="0.2">
       <c r="B124" s="25"/>
       <c r="D124" s="10"/>
       <c r="E124" s="21"/>
@@ -17229,7 +17280,7 @@
       <c r="BV124" s="10"/>
       <c r="BW124" s="10"/>
     </row>
-    <row r="125" spans="1:123">
+    <row r="125" spans="1:123" x14ac:dyDescent="0.2">
       <c r="B125" s="25"/>
       <c r="D125" s="10"/>
       <c r="E125" s="21"/>
@@ -17304,7 +17355,7 @@
       <c r="BV125" s="10"/>
       <c r="BW125" s="10"/>
     </row>
-    <row r="126" spans="1:123">
+    <row r="126" spans="1:123" x14ac:dyDescent="0.2">
       <c r="B126" s="25"/>
       <c r="D126" s="10"/>
       <c r="E126" s="21"/>
@@ -17379,7 +17430,7 @@
       <c r="BV126" s="10"/>
       <c r="BW126" s="10"/>
     </row>
-    <row r="127" spans="1:123">
+    <row r="127" spans="1:123" x14ac:dyDescent="0.2">
       <c r="B127" s="25"/>
       <c r="D127" s="10"/>
       <c r="E127" s="21"/>
@@ -17454,7 +17505,7 @@
       <c r="BV127" s="10"/>
       <c r="BW127" s="10"/>
     </row>
-    <row r="128" spans="1:123">
+    <row r="128" spans="1:123" x14ac:dyDescent="0.2">
       <c r="B128" s="25"/>
       <c r="D128" s="10"/>
       <c r="E128" s="21"/>
@@ -17529,7 +17580,7 @@
       <c r="BV128" s="10"/>
       <c r="BW128" s="10"/>
     </row>
-    <row r="129" spans="2:75">
+    <row r="129" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B129" s="25"/>
       <c r="D129" s="10"/>
       <c r="E129" s="21"/>
@@ -17604,7 +17655,7 @@
       <c r="BV129" s="10"/>
       <c r="BW129" s="10"/>
     </row>
-    <row r="130" spans="2:75">
+    <row r="130" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B130" s="25"/>
       <c r="D130" s="10"/>
       <c r="E130" s="21"/>
@@ -17679,7 +17730,7 @@
       <c r="BV130" s="10"/>
       <c r="BW130" s="10"/>
     </row>
-    <row r="131" spans="2:75">
+    <row r="131" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B131" s="25"/>
       <c r="D131" s="10"/>
       <c r="E131" s="21"/>
@@ -17754,7 +17805,7 @@
       <c r="BV131" s="10"/>
       <c r="BW131" s="10"/>
     </row>
-    <row r="132" spans="2:75">
+    <row r="132" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B132" s="25"/>
       <c r="D132" s="10"/>
       <c r="E132" s="21"/>
@@ -17829,7 +17880,7 @@
       <c r="BV132" s="10"/>
       <c r="BW132" s="10"/>
     </row>
-    <row r="133" spans="2:75">
+    <row r="133" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B133" s="25"/>
       <c r="D133" s="10"/>
       <c r="E133" s="21"/>
@@ -17904,7 +17955,7 @@
       <c r="BV133" s="10"/>
       <c r="BW133" s="10"/>
     </row>
-    <row r="134" spans="2:75">
+    <row r="134" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B134" s="25"/>
       <c r="D134" s="10"/>
       <c r="E134" s="21"/>
@@ -17979,7 +18030,7 @@
       <c r="BV134" s="10"/>
       <c r="BW134" s="10"/>
     </row>
-    <row r="135" spans="2:75">
+    <row r="135" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B135" s="25"/>
       <c r="D135" s="10"/>
       <c r="E135" s="21"/>
@@ -18054,7 +18105,7 @@
       <c r="BV135" s="10"/>
       <c r="BW135" s="10"/>
     </row>
-    <row r="136" spans="2:75">
+    <row r="136" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B136" s="25"/>
       <c r="D136" s="10"/>
       <c r="E136" s="21"/>
@@ -18129,7 +18180,7 @@
       <c r="BV136" s="10"/>
       <c r="BW136" s="10"/>
     </row>
-    <row r="137" spans="2:75">
+    <row r="137" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B137" s="25"/>
       <c r="D137" s="10"/>
       <c r="E137" s="21"/>
@@ -18204,7 +18255,7 @@
       <c r="BV137" s="10"/>
       <c r="BW137" s="10"/>
     </row>
-    <row r="138" spans="2:75">
+    <row r="138" spans="2:75" x14ac:dyDescent="0.2">
       <c r="B138" s="25"/>
       <c r="D138" s="10"/>
       <c r="E138" s="21"/>
@@ -18279,7 +18330,7 @@
       <c r="BV138" s="10"/>
       <c r="BW138" s="10"/>
     </row>
-    <row r="139" spans="2:75">
+    <row r="139" spans="2:75" x14ac:dyDescent="0.2">
       <c r="D139" s="10"/>
       <c r="E139" s="21"/>
       <c r="F139" s="10"/>
@@ -18353,7 +18404,7 @@
       <c r="BV139" s="10"/>
       <c r="BW139" s="10"/>
     </row>
-    <row r="140" spans="2:75">
+    <row r="140" spans="2:75" x14ac:dyDescent="0.2">
       <c r="D140" s="10"/>
       <c r="E140" s="21"/>
       <c r="F140" s="10"/>
@@ -18427,7 +18478,7 @@
       <c r="BV140" s="10"/>
       <c r="BW140" s="10"/>
     </row>
-    <row r="141" spans="2:75">
+    <row r="141" spans="2:75" x14ac:dyDescent="0.2">
       <c r="D141" s="10"/>
       <c r="E141" s="21"/>
       <c r="F141" s="10"/>
@@ -18501,7 +18552,7 @@
       <c r="BV141" s="10"/>
       <c r="BW141" s="10"/>
     </row>
-    <row r="142" spans="2:75">
+    <row r="142" spans="2:75" x14ac:dyDescent="0.2">
       <c r="D142" s="10"/>
       <c r="E142" s="21"/>
       <c r="F142" s="10"/>
@@ -18575,7 +18626,7 @@
       <c r="BV142" s="10"/>
       <c r="BW142" s="10"/>
     </row>
-    <row r="143" spans="2:75">
+    <row r="143" spans="2:75" x14ac:dyDescent="0.2">
       <c r="D143" s="10"/>
       <c r="E143" s="21"/>
       <c r="F143" s="10"/>
@@ -18649,7 +18700,7 @@
       <c r="BV143" s="10"/>
       <c r="BW143" s="10"/>
     </row>
-    <row r="144" spans="2:75">
+    <row r="144" spans="2:75" x14ac:dyDescent="0.2">
       <c r="D144" s="10"/>
       <c r="E144" s="21"/>
       <c r="F144" s="10"/>
@@ -18723,7 +18774,7 @@
       <c r="BV144" s="10"/>
       <c r="BW144" s="10"/>
     </row>
-    <row r="145" spans="4:75">
+    <row r="145" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D145" s="10"/>
       <c r="E145" s="21"/>
       <c r="F145" s="10"/>
@@ -18797,7 +18848,7 @@
       <c r="BV145" s="10"/>
       <c r="BW145" s="10"/>
     </row>
-    <row r="146" spans="4:75">
+    <row r="146" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D146" s="10"/>
       <c r="E146" s="21"/>
       <c r="F146" s="10"/>
@@ -18871,7 +18922,7 @@
       <c r="BV146" s="10"/>
       <c r="BW146" s="10"/>
     </row>
-    <row r="147" spans="4:75">
+    <row r="147" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D147" s="10"/>
       <c r="E147" s="21"/>
       <c r="F147" s="10"/>
@@ -18945,7 +18996,7 @@
       <c r="BV147" s="10"/>
       <c r="BW147" s="10"/>
     </row>
-    <row r="148" spans="4:75">
+    <row r="148" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D148" s="10"/>
       <c r="E148" s="21"/>
       <c r="F148" s="10"/>
@@ -19019,7 +19070,7 @@
       <c r="BV148" s="10"/>
       <c r="BW148" s="10"/>
     </row>
-    <row r="149" spans="4:75">
+    <row r="149" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D149" s="10"/>
       <c r="E149" s="21"/>
       <c r="F149" s="10"/>
@@ -19093,7 +19144,7 @@
       <c r="BV149" s="10"/>
       <c r="BW149" s="10"/>
     </row>
-    <row r="150" spans="4:75">
+    <row r="150" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D150" s="10"/>
       <c r="E150" s="21"/>
       <c r="F150" s="10"/>
@@ -19167,7 +19218,7 @@
       <c r="BV150" s="10"/>
       <c r="BW150" s="10"/>
     </row>
-    <row r="151" spans="4:75">
+    <row r="151" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D151" s="10"/>
       <c r="E151" s="21"/>
       <c r="F151" s="10"/>
@@ -19241,7 +19292,7 @@
       <c r="BV151" s="10"/>
       <c r="BW151" s="10"/>
     </row>
-    <row r="152" spans="4:75">
+    <row r="152" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D152" s="10"/>
       <c r="E152" s="21"/>
       <c r="F152" s="10"/>
@@ -19315,7 +19366,7 @@
       <c r="BV152" s="10"/>
       <c r="BW152" s="10"/>
     </row>
-    <row r="153" spans="4:75">
+    <row r="153" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D153" s="10"/>
       <c r="E153" s="21"/>
       <c r="F153" s="10"/>
@@ -19389,7 +19440,7 @@
       <c r="BV153" s="10"/>
       <c r="BW153" s="10"/>
     </row>
-    <row r="154" spans="4:75">
+    <row r="154" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D154" s="10"/>
       <c r="E154" s="21"/>
       <c r="F154" s="10"/>
@@ -19463,7 +19514,7 @@
       <c r="BV154" s="10"/>
       <c r="BW154" s="10"/>
     </row>
-    <row r="155" spans="4:75">
+    <row r="155" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D155" s="10"/>
       <c r="E155" s="21"/>
       <c r="F155" s="10"/>
@@ -19537,7 +19588,7 @@
       <c r="BV155" s="10"/>
       <c r="BW155" s="10"/>
     </row>
-    <row r="156" spans="4:75">
+    <row r="156" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D156" s="10"/>
       <c r="E156" s="21"/>
       <c r="F156" s="10"/>
@@ -19611,7 +19662,7 @@
       <c r="BV156" s="10"/>
       <c r="BW156" s="10"/>
     </row>
-    <row r="157" spans="4:75">
+    <row r="157" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D157" s="10"/>
       <c r="E157" s="21"/>
       <c r="F157" s="10"/>
@@ -19685,7 +19736,7 @@
       <c r="BV157" s="10"/>
       <c r="BW157" s="10"/>
     </row>
-    <row r="158" spans="4:75">
+    <row r="158" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D158" s="10"/>
       <c r="E158" s="21"/>
       <c r="F158" s="10"/>
@@ -19759,7 +19810,7 @@
       <c r="BV158" s="10"/>
       <c r="BW158" s="10"/>
     </row>
-    <row r="159" spans="4:75">
+    <row r="159" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D159" s="10"/>
       <c r="E159" s="21"/>
       <c r="F159" s="10"/>
@@ -19833,7 +19884,7 @@
       <c r="BV159" s="10"/>
       <c r="BW159" s="10"/>
     </row>
-    <row r="160" spans="4:75">
+    <row r="160" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D160" s="10"/>
       <c r="E160" s="21"/>
       <c r="F160" s="10"/>
@@ -19907,7 +19958,7 @@
       <c r="BV160" s="10"/>
       <c r="BW160" s="10"/>
     </row>
-    <row r="161" spans="4:75">
+    <row r="161" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D161" s="10"/>
       <c r="E161" s="21"/>
       <c r="F161" s="10"/>
@@ -19981,7 +20032,7 @@
       <c r="BV161" s="10"/>
       <c r="BW161" s="10"/>
     </row>
-    <row r="162" spans="4:75">
+    <row r="162" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D162" s="10"/>
       <c r="E162" s="21"/>
       <c r="F162" s="10"/>
@@ -20055,7 +20106,7 @@
       <c r="BV162" s="10"/>
       <c r="BW162" s="10"/>
     </row>
-    <row r="163" spans="4:75">
+    <row r="163" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D163" s="10"/>
       <c r="E163" s="21"/>
       <c r="F163" s="10"/>
@@ -20129,7 +20180,7 @@
       <c r="BV163" s="10"/>
       <c r="BW163" s="10"/>
     </row>
-    <row r="164" spans="4:75">
+    <row r="164" spans="4:75" x14ac:dyDescent="0.2">
       <c r="D164" s="10"/>
       <c r="E164" s="21"/>
       <c r="F164" s="10"/>
@@ -20216,10 +20267,5 @@
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding template to demonstrate PGP Encrypt/Decrypt. Credit to Andrew LoPresto.
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="195">
   <si>
     <t>Template Name:</t>
   </si>
@@ -612,6 +612,13 @@
   </si>
   <si>
     <t>This template downloads an index of xml documents from an HTML page, then prioritize the downloads of different linked pages, and controls the rate of download, before extracting, de-duplicating and routing the results.</t>
+  </si>
+  <si>
+    <t>PGP Encryption Test</t>
+  </si>
+  <si>
+    <t>Generates empty flowfiles, replaces the contents with a static plaintext message, and writes them as a file to a directory. 
+Reads files from a directory, encrypts using PGP, logs, decrypts, and writes the plaintext files to a new directory.</t>
   </si>
 </sst>
 </file>
@@ -1390,10 +1397,10 @@
   <dimension ref="A1:DT164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="CF30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="K39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="DS31" sqref="DS31"/>
+      <selection pane="bottomRight" activeCell="K40" sqref="K40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1513,7 +1520,7 @@
       </c>
       <c r="AD1">
         <f t="shared" si="1"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AE1">
         <f t="shared" si="1"/>
@@ -1585,7 +1592,7 @@
       </c>
       <c r="AW1">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AX1">
         <f t="shared" si="1"/>
@@ -1593,7 +1600,7 @@
       </c>
       <c r="AY1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AZ1">
         <f t="shared" si="1"/>
@@ -1697,7 +1704,7 @@
       </c>
       <c r="BZ1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="CA1">
         <f t="shared" si="1"/>
@@ -1733,7 +1740,7 @@
       </c>
       <c r="CI1">
         <f t="shared" ref="CI1:DS1" si="2">COUNTIFS(CI10:CI300,"X")</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="CJ1">
         <f t="shared" si="2"/>
@@ -1793,7 +1800,7 @@
       </c>
       <c r="CX1">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="CY1">
         <f t="shared" si="2"/>
@@ -1869,7 +1876,7 @@
       </c>
       <c r="DQ1">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="DR1">
         <f t="shared" si="2"/>
@@ -7120,7 +7127,7 @@
       <c r="O40" s="13"/>
       <c r="P40" s="13"/>
       <c r="Q40" s="13" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
       <c r="R40" s="13"/>
       <c r="S40" s="13"/>
@@ -7132,7 +7139,7 @@
       <c r="Y40" s="13"/>
       <c r="Z40" s="13"/>
       <c r="AA40" s="13" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
       <c r="AB40" s="13"/>
       <c r="AC40" s="13"/>
@@ -7141,7 +7148,7 @@
       <c r="AF40" s="13"/>
       <c r="AG40" s="13"/>
       <c r="AH40" s="13" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
       <c r="AI40" s="13"/>
       <c r="AJ40" s="13"/>
@@ -7153,7 +7160,7 @@
       <c r="AP40" s="13"/>
       <c r="AQ40" s="13"/>
       <c r="AR40" s="13" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
       <c r="AS40" s="13"/>
       <c r="AT40" s="13"/>
@@ -7162,14 +7169,14 @@
       <c r="AW40" s="13"/>
       <c r="AX40" s="13"/>
       <c r="AY40" s="13" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
       <c r="AZ40" s="13"/>
       <c r="BA40" s="13"/>
       <c r="BB40" s="13"/>
       <c r="BC40" s="13"/>
       <c r="BD40" s="13" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
       <c r="BE40" s="13"/>
       <c r="BF40" s="13"/>
@@ -7183,11 +7190,11 @@
       <c r="BN40" s="13"/>
       <c r="BO40" s="13"/>
       <c r="BP40" s="13" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
       <c r="BQ40" s="13"/>
       <c r="BR40" s="13" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
       <c r="BS40" s="13"/>
       <c r="BT40" s="13"/>
@@ -7206,7 +7213,7 @@
       <c r="CG40" s="13"/>
       <c r="CH40" s="13"/>
       <c r="CI40" s="13" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
       <c r="CJ40" s="13"/>
       <c r="CK40" s="13"/>
@@ -7214,7 +7221,7 @@
       <c r="CM40" s="13"/>
       <c r="CN40" s="13"/>
       <c r="CO40" s="13" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
       <c r="CP40" s="13"/>
       <c r="CQ40" s="13"/>
@@ -7232,7 +7239,7 @@
       <c r="DC40" s="13"/>
       <c r="DD40" s="13"/>
       <c r="DE40" s="13" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
       <c r="DF40" s="13"/>
       <c r="DG40" s="13"/>
@@ -7246,14 +7253,18 @@
       <c r="DO40" s="13"/>
       <c r="DP40" s="13"/>
       <c r="DQ40" s="13" t="s">
-        <v>191</v>
+        <v>27</v>
       </c>
       <c r="DR40" s="13"/>
       <c r="DS40" s="13"/>
     </row>
     <row r="41" spans="1:123" ht="72" customHeight="1">
-      <c r="A41" s="16"/>
-      <c r="B41" s="24"/>
+      <c r="A41" s="16" t="s">
+        <v>193</v>
+      </c>
+      <c r="B41" s="24" t="s">
+        <v>194</v>
+      </c>
       <c r="D41" s="18"/>
       <c r="E41" s="18"/>
       <c r="F41" s="13"/>
@@ -7280,7 +7291,9 @@
       <c r="AA41" s="13"/>
       <c r="AB41" s="13"/>
       <c r="AC41" s="13"/>
-      <c r="AD41" s="13"/>
+      <c r="AD41" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="AE41" s="13"/>
       <c r="AF41" s="13"/>
       <c r="AG41" s="13"/>
@@ -7299,9 +7312,13 @@
       <c r="AT41" s="13"/>
       <c r="AU41" s="13"/>
       <c r="AV41" s="13"/>
-      <c r="AW41" s="13"/>
+      <c r="AW41" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="AX41" s="13"/>
-      <c r="AY41" s="13"/>
+      <c r="AY41" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="AZ41" s="13"/>
       <c r="BA41" s="13"/>
       <c r="BB41" s="13"/>
@@ -7328,7 +7345,9 @@
       <c r="BW41" s="13"/>
       <c r="BX41" s="13"/>
       <c r="BY41" s="13"/>
-      <c r="BZ41" s="13"/>
+      <c r="BZ41" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CA41" s="13"/>
       <c r="CB41" s="13"/>
       <c r="CC41" s="13"/>
@@ -7337,7 +7356,9 @@
       <c r="CF41" s="13"/>
       <c r="CG41" s="13"/>
       <c r="CH41" s="13"/>
-      <c r="CI41" s="13"/>
+      <c r="CI41" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CJ41" s="13"/>
       <c r="CK41" s="13"/>
       <c r="CL41" s="13"/>
@@ -7352,7 +7373,9 @@
       <c r="CU41" s="13"/>
       <c r="CV41" s="13"/>
       <c r="CW41" s="13"/>
-      <c r="CX41" s="13"/>
+      <c r="CX41" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CY41" s="13"/>
       <c r="CZ41" s="13"/>
       <c r="DA41" s="13"/>
@@ -7371,7 +7394,9 @@
       <c r="DN41" s="13"/>
       <c r="DO41" s="13"/>
       <c r="DP41" s="13"/>
-      <c r="DQ41" s="13"/>
+      <c r="DQ41" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="DR41" s="13"/>
       <c r="DS41" s="13"/>
     </row>

</xml_diff>

<commit_message>
Adding Ambari report handler template
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="197">
   <si>
     <t>Template Name:</t>
   </si>
@@ -619,6 +619,12 @@
   <si>
     <t>Generates empty flowfiles, replaces the contents with a static plaintext message, and writes them as a file to a directory. 
 Reads files from a directory, encrypts using PGP, logs, decrypts, and writes the plaintext files to a new directory.</t>
+  </si>
+  <si>
+    <t>HandleNifiReports</t>
+  </si>
+  <si>
+    <t>Receive and handle Ambari reports.</t>
   </si>
 </sst>
 </file>
@@ -1397,10 +1403,10 @@
   <dimension ref="A1:DT164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="K39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="CF39" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="K40" sqref="K40"/>
+      <selection pane="bottomRight" activeCell="DQ42" sqref="DQ42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1448,7 +1454,7 @@
       </c>
       <c r="K1">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L1">
         <f t="shared" si="0"/>
@@ -1524,7 +1530,7 @@
       </c>
       <c r="AE1">
         <f t="shared" si="1"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AF1">
         <f t="shared" si="1"/>
@@ -1656,11 +1662,11 @@
       </c>
       <c r="BM1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BN1">
         <f t="shared" si="1"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="BO1">
         <f t="shared" si="1"/>
@@ -1704,7 +1710,7 @@
       </c>
       <c r="BZ1">
         <f t="shared" si="1"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="CA1">
         <f t="shared" si="1"/>
@@ -1848,7 +1854,7 @@
       </c>
       <c r="DJ1">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="DK1">
         <f t="shared" si="2"/>
@@ -1876,7 +1882,7 @@
       </c>
       <c r="DQ1">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="DR1">
         <f t="shared" si="2"/>
@@ -7401,8 +7407,12 @@
       <c r="DS41" s="13"/>
     </row>
     <row r="42" spans="1:123" ht="72" customHeight="1">
-      <c r="A42" s="16"/>
-      <c r="B42" s="24"/>
+      <c r="A42" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="B42" s="24" t="s">
+        <v>196</v>
+      </c>
       <c r="D42" s="18"/>
       <c r="E42" s="18"/>
       <c r="F42" s="13"/>
@@ -7410,7 +7420,9 @@
       <c r="H42" s="13"/>
       <c r="I42" s="13"/>
       <c r="J42" s="13"/>
-      <c r="K42" s="13"/>
+      <c r="K42" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="L42" s="13"/>
       <c r="M42" s="14"/>
       <c r="N42" s="13"/>
@@ -7430,7 +7442,9 @@
       <c r="AB42" s="13"/>
       <c r="AC42" s="13"/>
       <c r="AD42" s="13"/>
-      <c r="AE42" s="13"/>
+      <c r="AE42" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="AF42" s="13"/>
       <c r="AG42" s="13"/>
       <c r="AH42" s="13"/>
@@ -7464,8 +7478,12 @@
       <c r="BJ42" s="13"/>
       <c r="BK42" s="13"/>
       <c r="BL42" s="13"/>
-      <c r="BM42" s="13"/>
-      <c r="BN42" s="13"/>
+      <c r="BM42" s="13" t="s">
+        <v>27</v>
+      </c>
+      <c r="BN42" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="BO42" s="13"/>
       <c r="BP42" s="13"/>
       <c r="BQ42" s="13"/>
@@ -7477,7 +7495,9 @@
       <c r="BW42" s="13"/>
       <c r="BX42" s="13"/>
       <c r="BY42" s="13"/>
-      <c r="BZ42" s="13"/>
+      <c r="BZ42" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CA42" s="13"/>
       <c r="CB42" s="13"/>
       <c r="CC42" s="13"/>
@@ -7513,14 +7533,18 @@
       <c r="DG42" s="13"/>
       <c r="DH42" s="13"/>
       <c r="DI42" s="13"/>
-      <c r="DJ42" s="13"/>
+      <c r="DJ42" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="DK42" s="13"/>
       <c r="DL42" s="13"/>
       <c r="DM42" s="13"/>
       <c r="DN42" s="13"/>
       <c r="DO42" s="13"/>
       <c r="DP42" s="13"/>
-      <c r="DQ42" s="13"/>
+      <c r="DQ42" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="DR42" s="13"/>
       <c r="DS42" s="13"/>
     </row>

</xml_diff>

<commit_message>
Adding a simple example using the ReplaceTextWithMapping processor. Credit to Jeremy Dyer.
</commit_message>
<xml_diff>
--- a/NiFi Templates.xlsx
+++ b/NiFi Templates.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="448" uniqueCount="199">
   <si>
     <t>Template Name:</t>
   </si>
@@ -625,6 +625,12 @@
   </si>
   <si>
     <t>Receive and handle Ambari reports.</t>
+  </si>
+  <si>
+    <t>ReplaceTextWithMapping-Example</t>
+  </si>
+  <si>
+    <t>A simple example flow utiliizing the ReplaceTextWithMapping processor. This uses the mapping file in the resources folder of this repo.The format for the mapping file is newline delimited per mapping defined with a \t character separator the mapping key to the desired replacement value. </t>
   </si>
 </sst>
 </file>
@@ -1403,10 +1409,10 @@
   <dimension ref="A1:DT164"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="8" topLeftCell="CF39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="8" topLeftCell="CC40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="DQ42" sqref="DQ42"/>
+      <selection pane="bottomRight" activeCell="DQ43" sqref="DQ43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1606,7 +1612,7 @@
       </c>
       <c r="AY1">
         <f t="shared" si="1"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="AZ1">
         <f t="shared" si="1"/>
@@ -1746,7 +1752,7 @@
       </c>
       <c r="CI1">
         <f t="shared" ref="CI1:DS1" si="2">COUNTIFS(CI10:CI300,"X")</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="CJ1">
         <f t="shared" si="2"/>
@@ -1810,7 +1816,7 @@
       </c>
       <c r="CY1">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CZ1">
         <f t="shared" si="2"/>
@@ -1882,7 +1888,7 @@
       </c>
       <c r="DQ1">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="DR1">
         <f t="shared" si="2"/>
@@ -7549,8 +7555,12 @@
       <c r="DS42" s="13"/>
     </row>
     <row r="43" spans="1:123" ht="72" customHeight="1">
-      <c r="A43" s="16"/>
-      <c r="B43" s="24"/>
+      <c r="A43" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="B43" s="24" t="s">
+        <v>198</v>
+      </c>
       <c r="D43" s="18"/>
       <c r="E43" s="18"/>
       <c r="F43" s="13"/>
@@ -7598,7 +7608,9 @@
       <c r="AV43" s="13"/>
       <c r="AW43" s="13"/>
       <c r="AX43" s="13"/>
-      <c r="AY43" s="13"/>
+      <c r="AY43" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="AZ43" s="13"/>
       <c r="BA43" s="13"/>
       <c r="BB43" s="13"/>
@@ -7634,7 +7646,9 @@
       <c r="CF43" s="13"/>
       <c r="CG43" s="13"/>
       <c r="CH43" s="13"/>
-      <c r="CI43" s="13"/>
+      <c r="CI43" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CJ43" s="13"/>
       <c r="CK43" s="13"/>
       <c r="CL43" s="13"/>
@@ -7650,7 +7664,9 @@
       <c r="CV43" s="13"/>
       <c r="CW43" s="13"/>
       <c r="CX43" s="13"/>
-      <c r="CY43" s="13"/>
+      <c r="CY43" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="CZ43" s="13"/>
       <c r="DA43" s="13"/>
       <c r="DB43" s="13"/>
@@ -7668,7 +7684,9 @@
       <c r="DN43" s="13"/>
       <c r="DO43" s="13"/>
       <c r="DP43" s="13"/>
-      <c r="DQ43" s="13"/>
+      <c r="DQ43" s="13" t="s">
+        <v>27</v>
+      </c>
       <c r="DR43" s="13"/>
       <c r="DS43" s="13"/>
     </row>

</xml_diff>